<commit_message>
decreased data set size to speed up debugging
</commit_message>
<xml_diff>
--- a/data/amazon_test_big.xlsx
+++ b/data/amazon_test_big.xlsx
@@ -5,22 +5,23 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="973" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SKU_ASIN" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">MAIN!$A$1:$D$795</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">MAIN!$A$1:$D$10</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">MAIN!$A$1:$D$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">MAIN!$A$1:$D$789</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">MAIN!$A$1:$D$10</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="110">
   <si>
     <t>Model #</t>
   </si>
@@ -50,42 +51,6 @@
   </si>
   <si>
     <t>B0035C67XE</t>
-  </si>
-  <si>
-    <t>Buckingham</t>
-  </si>
-  <si>
-    <t>B003G589YA</t>
-  </si>
-  <si>
-    <t>Cheshire</t>
-  </si>
-  <si>
-    <t>B003G51G86</t>
-  </si>
-  <si>
-    <t>Cornwall</t>
-  </si>
-  <si>
-    <t>B0021MU6WM</t>
-  </si>
-  <si>
-    <t>Derbyshire</t>
-  </si>
-  <si>
-    <t>B005UW7970</t>
-  </si>
-  <si>
-    <t>Cumberland</t>
-  </si>
-  <si>
-    <t>B0021MNJ9E</t>
-  </si>
-  <si>
-    <t>Durham</t>
-  </si>
-  <si>
-    <t>B003G55KJM</t>
   </si>
   <si>
     <t>SKU</t>
@@ -587,7 +552,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
       <border diagonalUp="false" diagonalDown="false">
@@ -611,10 +576,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -683,100 +648,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>20206</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>715709275849</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>20484</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>715709288290</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
-        <v>20485</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>715709288795</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>20542</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>715709289471</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
-        <v>20544</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>715709288948</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>20639</v>
-      </c>
-      <c r="B10" s="5" t="n">
-        <v>715709297421</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D795"/>
-  <conditionalFormatting sqref="A11">
+  <autoFilter ref="A1:D10"/>
+  <conditionalFormatting sqref="A5">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>OR(C602=7)</formula>
+      <formula>OR(C596=7)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
+  <conditionalFormatting sqref="A5">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>OR(C602=6)</formula>
+      <formula>OR(C596=6)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -795,7 +676,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z107"/>
+  <dimension ref="A1:Z101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A799" activeCellId="0" sqref="A799"/>
@@ -812,13 +693,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -849,7 +730,7 @@
         <v>6705</v>
       </c>
       <c r="B2" s="10" t="str">
-        <f aca="false">VLOOKUP(A2,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A2,MAIN!A$1:D$1047785,4,0)</f>
         <v>B0021MU9HE</v>
       </c>
       <c r="C2" s="9" t="n">
@@ -861,7 +742,7 @@
         <v>6715</v>
       </c>
       <c r="B3" s="10" t="str">
-        <f aca="false">VLOOKUP(A3,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A3,MAIN!A$1:D$1047785,4,0)</f>
         <v>B001I6OGIM</v>
       </c>
       <c r="C3" s="9" t="n">
@@ -873,7 +754,7 @@
         <v>20205</v>
       </c>
       <c r="B4" s="10" t="str">
-        <f aca="false">VLOOKUP(A4,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A4,MAIN!A$1:D$1047785,4,0)</f>
         <v>B0035C67XE</v>
       </c>
       <c r="C4" s="9" t="n">
@@ -881,159 +762,297 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
-        <v>20206</v>
-      </c>
-      <c r="B5" s="10" t="str">
-        <f aca="false">VLOOKUP(A5,MAIN!A$1:D$1047791,4,0)</f>
-        <v>B003G589YA</v>
-      </c>
-      <c r="C5" s="9" t="n">
-        <v>20206</v>
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10" t="e">
+        <f aca="false">VLOOKUP(A5,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="n">
-        <v>20484</v>
-      </c>
-      <c r="B6" s="10" t="str">
-        <f aca="false">VLOOKUP(A6,MAIN!A$1:D$1047791,4,0)</f>
-        <v>B003G51G86</v>
-      </c>
-      <c r="C6" s="9" t="n">
-        <v>20484</v>
+      <c r="A6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="10" t="e">
+        <f aca="false">VLOOKUP(A6,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="n">
-        <v>20485</v>
-      </c>
-      <c r="B7" s="10" t="str">
-        <f aca="false">VLOOKUP(A7,MAIN!A$1:D$1047791,4,0)</f>
-        <v>B0021MU6WM</v>
-      </c>
-      <c r="C7" s="9" t="n">
-        <v>20485</v>
+      <c r="A7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="10" t="e">
+        <f aca="false">VLOOKUP(A7,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="n">
-        <v>20542</v>
-      </c>
-      <c r="B8" s="10" t="str">
-        <f aca="false">VLOOKUP(A8,MAIN!A$1:D$1047791,4,0)</f>
-        <v>B005UW7970</v>
-      </c>
-      <c r="C8" s="9" t="n">
-        <v>20542</v>
+      <c r="A8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="10" t="e">
+        <f aca="false">VLOOKUP(A8,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="n">
-        <v>20544</v>
-      </c>
-      <c r="B9" s="10" t="str">
-        <f aca="false">VLOOKUP(A9,MAIN!A$1:D$1047791,4,0)</f>
-        <v>B0021MNJ9E</v>
-      </c>
-      <c r="C9" s="9" t="n">
-        <v>20544</v>
+      <c r="A9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="10" t="e">
+        <f aca="false">VLOOKUP(A9,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="n">
-        <v>20639</v>
-      </c>
-      <c r="B10" s="10" t="str">
-        <f aca="false">VLOOKUP(A10,MAIN!A$1:D$1047791,4,0)</f>
-        <v>B003G55KJM</v>
-      </c>
-      <c r="C10" s="9" t="n">
-        <v>20639</v>
+      <c r="A10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="10" t="e">
+        <f aca="false">VLOOKUP(A10,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10" t="e">
-        <f aca="false">VLOOKUP(A11,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A11,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B12" s="10" t="e">
-        <f aca="false">VLOOKUP(A12,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A12,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B13" s="10" t="e">
-        <f aca="false">VLOOKUP(A13,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A13,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B14" s="10" t="e">
-        <f aca="false">VLOOKUP(A14,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A14,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B15" s="10" t="e">
-        <f aca="false">VLOOKUP(A15,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A15,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B16" s="10" t="e">
-        <f aca="false">VLOOKUP(A16,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A16,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B17" s="10" t="e">
-        <f aca="false">VLOOKUP(A17,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A17,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -1061,14 +1080,14 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B18" s="10" t="e">
-        <f aca="false">VLOOKUP(A18,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A18,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -1096,14 +1115,14 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B19" s="10" t="e">
-        <f aca="false">VLOOKUP(A19,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A19,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1131,14 +1150,14 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B20" s="10" t="e">
-        <f aca="false">VLOOKUP(A20,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A20,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -1166,14 +1185,14 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B21" s="10" t="e">
-        <f aca="false">VLOOKUP(A21,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A21,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -1201,14 +1220,14 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B22" s="10" t="e">
-        <f aca="false">VLOOKUP(A22,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A22,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1236,14 +1255,14 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B23" s="10" t="e">
-        <f aca="false">VLOOKUP(A23,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A23,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1271,14 +1290,14 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B24" s="10" t="e">
-        <f aca="false">VLOOKUP(A24,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A24,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -1306,14 +1325,14 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B25" s="10" t="e">
-        <f aca="false">VLOOKUP(A25,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A25,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1341,14 +1360,14 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B26" s="10" t="e">
-        <f aca="false">VLOOKUP(A26,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A26,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1376,14 +1395,14 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B27" s="10" t="e">
-        <f aca="false">VLOOKUP(A27,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A27,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1411,14 +1430,14 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B28" s="10" t="e">
-        <f aca="false">VLOOKUP(A28,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A28,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -1446,14 +1465,14 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B29" s="10" t="e">
-        <f aca="false">VLOOKUP(A29,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A29,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -1481,14 +1500,14 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B30" s="10" t="e">
-        <f aca="false">VLOOKUP(A30,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A30,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -1516,14 +1535,14 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B31" s="10" t="e">
-        <f aca="false">VLOOKUP(A31,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A31,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -1551,14 +1570,14 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B32" s="10" t="e">
-        <f aca="false">VLOOKUP(A32,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A32,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -1586,14 +1605,14 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B33" s="10" t="e">
-        <f aca="false">VLOOKUP(A33,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A33,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -1621,14 +1640,14 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B34" s="10" t="e">
-        <f aca="false">VLOOKUP(A34,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A34,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -1656,14 +1675,14 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B35" s="10" t="e">
-        <f aca="false">VLOOKUP(A35,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A35,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -1691,14 +1710,14 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B36" s="10" t="e">
-        <f aca="false">VLOOKUP(A36,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A36,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -1726,14 +1745,14 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B37" s="10" t="e">
-        <f aca="false">VLOOKUP(A37,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A37,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -1761,14 +1780,14 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B38" s="10" t="e">
-        <f aca="false">VLOOKUP(A38,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A38,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -1796,14 +1815,14 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B39" s="10" t="e">
-        <f aca="false">VLOOKUP(A39,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A39,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -1831,14 +1850,14 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B40" s="10" t="e">
-        <f aca="false">VLOOKUP(A40,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A40,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -1866,14 +1885,14 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B41" s="10" t="e">
-        <f aca="false">VLOOKUP(A41,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A41,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -1901,14 +1920,14 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B42" s="10" t="e">
-        <f aca="false">VLOOKUP(A42,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A42,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -1936,14 +1955,14 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B43" s="10" t="e">
-        <f aca="false">VLOOKUP(A43,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A43,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -1971,14 +1990,14 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B44" s="10" t="e">
-        <f aca="false">VLOOKUP(A44,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A44,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -2006,14 +2025,14 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B45" s="10" t="e">
-        <f aca="false">VLOOKUP(A45,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A45,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -2041,15 +2060,13 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B46" s="10" t="e">
-        <f aca="false">VLOOKUP(A46,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>25</v>
-      </c>
+        <f aca="false">VLOOKUP(A46,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
@@ -2076,15 +2093,13 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B47" s="10" t="e">
-        <f aca="false">VLOOKUP(A47,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>25</v>
-      </c>
+        <f aca="false">VLOOKUP(A47,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
@@ -2111,15 +2126,13 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B48" s="10" t="e">
-        <f aca="false">VLOOKUP(A48,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>25</v>
-      </c>
+        <f aca="false">VLOOKUP(A48,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
@@ -2146,15 +2159,13 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B49" s="10" t="e">
-        <f aca="false">VLOOKUP(A49,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>25</v>
-      </c>
+        <f aca="false">VLOOKUP(A49,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
@@ -2181,15 +2192,13 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B50" s="10" t="e">
-        <f aca="false">VLOOKUP(A50,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>25</v>
-      </c>
+        <f aca="false">VLOOKUP(A50,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="9"/>
@@ -2216,15 +2225,13 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B51" s="10" t="e">
-        <f aca="false">VLOOKUP(A51,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>25</v>
-      </c>
+        <f aca="false">VLOOKUP(A51,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
@@ -2251,10 +2258,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B52" s="10" t="e">
-        <f aca="false">VLOOKUP(A52,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A52,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C52" s="9"/>
@@ -2284,10 +2291,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B53" s="10" t="e">
-        <f aca="false">VLOOKUP(A53,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A53,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C53" s="9"/>
@@ -2317,10 +2324,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B54" s="10" t="e">
-        <f aca="false">VLOOKUP(A54,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A54,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C54" s="9"/>
@@ -2350,10 +2357,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B55" s="10" t="e">
-        <f aca="false">VLOOKUP(A55,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A55,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C55" s="9"/>
@@ -2383,10 +2390,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B56" s="10" t="e">
-        <f aca="false">VLOOKUP(A56,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A56,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C56" s="9"/>
@@ -2416,10 +2423,10 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B57" s="10" t="e">
-        <f aca="false">VLOOKUP(A57,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A57,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C57" s="9"/>
@@ -2449,10 +2456,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B58" s="10" t="e">
-        <f aca="false">VLOOKUP(A58,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A58,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C58" s="9"/>
@@ -2482,10 +2489,10 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B59" s="10" t="e">
-        <f aca="false">VLOOKUP(A59,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A59,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C59" s="9"/>
@@ -2515,13 +2522,15 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60" s="10" t="e">
-        <f aca="false">VLOOKUP(A60,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C60" s="9"/>
+        <v>68</v>
+      </c>
+      <c r="B60" s="9" t="e">
+        <f aca="false">VLOOKUP(A60,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="9"/>
@@ -2548,13 +2557,15 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B61" s="10" t="e">
-        <f aca="false">VLOOKUP(A61,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C61" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="B61" s="9" t="e">
+        <f aca="false">VLOOKUP(A61,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
@@ -2581,13 +2592,15 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B62" s="10" t="e">
-        <f aca="false">VLOOKUP(A62,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C62" s="9"/>
+        <v>70</v>
+      </c>
+      <c r="B62" s="9" t="e">
+        <f aca="false">VLOOKUP(A62,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
@@ -2614,13 +2627,15 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B63" s="10" t="e">
-        <f aca="false">VLOOKUP(A63,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C63" s="9"/>
+        <v>71</v>
+      </c>
+      <c r="B63" s="9" t="e">
+        <f aca="false">VLOOKUP(A63,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
       <c r="F63" s="9"/>
@@ -2647,13 +2662,15 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B64" s="10" t="e">
-        <f aca="false">VLOOKUP(A64,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C64" s="9"/>
+        <v>72</v>
+      </c>
+      <c r="B64" s="9" t="e">
+        <f aca="false">VLOOKUP(A64,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
       <c r="F64" s="9"/>
@@ -2680,13 +2697,15 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" s="10" t="e">
-        <f aca="false">VLOOKUP(A65,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C65" s="9"/>
+        <v>73</v>
+      </c>
+      <c r="B65" s="9" t="e">
+        <f aca="false">VLOOKUP(A65,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
       <c r="F65" s="9"/>
@@ -2713,14 +2732,14 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B66" s="9" t="e">
-        <f aca="false">VLOOKUP(A66,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A66,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
@@ -2748,14 +2767,14 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B67" s="9" t="e">
-        <f aca="false">VLOOKUP(A67,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A67,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
@@ -2783,14 +2802,14 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B68" s="9" t="e">
-        <f aca="false">VLOOKUP(A68,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A68,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
@@ -2818,14 +2837,14 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B69" s="9" t="e">
-        <f aca="false">VLOOKUP(A69,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A69,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -2853,14 +2872,14 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B70" s="9" t="e">
-        <f aca="false">VLOOKUP(A70,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A70,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
@@ -2888,14 +2907,14 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B71" s="9" t="e">
-        <f aca="false">VLOOKUP(A71,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A71,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
@@ -2923,14 +2942,14 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B72" s="9" t="e">
-        <f aca="false">VLOOKUP(A72,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A72,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -2958,14 +2977,14 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B73" s="9" t="e">
-        <f aca="false">VLOOKUP(A73,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A73,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -2993,14 +3012,14 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B74" s="9" t="e">
-        <f aca="false">VLOOKUP(A74,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A74,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -3028,14 +3047,14 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B75" s="9" t="e">
-        <f aca="false">VLOOKUP(A75,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A75,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
@@ -3063,14 +3082,14 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B76" s="9" t="e">
-        <f aca="false">VLOOKUP(A76,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A76,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
@@ -3098,14 +3117,14 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B77" s="9" t="e">
-        <f aca="false">VLOOKUP(A77,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A77,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
@@ -3133,14 +3152,14 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B78" s="9" t="e">
-        <f aca="false">VLOOKUP(A78,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A78,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
@@ -3168,14 +3187,14 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B79" s="9" t="e">
-        <f aca="false">VLOOKUP(A79,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A79,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
@@ -3203,14 +3222,14 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B80" s="9" t="e">
-        <f aca="false">VLOOKUP(A80,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A80,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
@@ -3238,14 +3257,14 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B81" s="9" t="e">
-        <f aca="false">VLOOKUP(A81,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A81,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
@@ -3273,15 +3292,13 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B82" s="9" t="e">
-        <f aca="false">VLOOKUP(A82,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B82" s="10" t="e">
+        <f aca="false">VLOOKUP(A82,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C82" s="9"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
@@ -3308,15 +3325,13 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B83" s="9" t="e">
-        <f aca="false">VLOOKUP(A83,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B83" s="10" t="e">
+        <f aca="false">VLOOKUP(A83,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
@@ -3343,15 +3358,13 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B84" s="9" t="e">
-        <f aca="false">VLOOKUP(A84,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B84" s="10" t="e">
+        <f aca="false">VLOOKUP(A84,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
@@ -3378,15 +3391,13 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B85" s="9" t="e">
-        <f aca="false">VLOOKUP(A85,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B85" s="10" t="e">
+        <f aca="false">VLOOKUP(A85,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C85" s="9"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
@@ -3413,15 +3424,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B86" s="9" t="e">
-        <f aca="false">VLOOKUP(A86,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B86" s="10" t="e">
+        <f aca="false">VLOOKUP(A86,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C86" s="9"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
@@ -3448,15 +3457,13 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B87" s="9" t="e">
-        <f aca="false">VLOOKUP(A87,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>25</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B87" s="10" t="e">
+        <f aca="false">VLOOKUP(A87,MAIN!A$1:D$1047785,4,0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="C87" s="9"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
@@ -3483,10 +3490,10 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B88" s="10" t="e">
-        <f aca="false">VLOOKUP(A88,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A88,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C88" s="9"/>
@@ -3516,10 +3523,10 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B89" s="10" t="e">
-        <f aca="false">VLOOKUP(A89,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A89,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C89" s="9"/>
@@ -3549,10 +3556,10 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B90" s="10" t="e">
-        <f aca="false">VLOOKUP(A90,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A90,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C90" s="9"/>
@@ -3582,10 +3589,10 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B91" s="10" t="e">
-        <f aca="false">VLOOKUP(A91,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A91,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C91" s="9"/>
@@ -3615,10 +3622,10 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B92" s="10" t="e">
-        <f aca="false">VLOOKUP(A92,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A92,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C92" s="9"/>
@@ -3648,10 +3655,10 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B93" s="10" t="e">
-        <f aca="false">VLOOKUP(A93,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A93,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C93" s="9"/>
@@ -3681,10 +3688,10 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B94" s="10" t="e">
-        <f aca="false">VLOOKUP(A94,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A94,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C94" s="9"/>
@@ -3714,10 +3721,10 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B95" s="10" t="e">
-        <f aca="false">VLOOKUP(A95,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A95,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C95" s="9"/>
@@ -3747,10 +3754,10 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B96" s="10" t="e">
-        <f aca="false">VLOOKUP(A96,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A96,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C96" s="9"/>
@@ -3780,10 +3787,10 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="9" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B97" s="10" t="e">
-        <f aca="false">VLOOKUP(A97,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A97,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C97" s="9"/>
@@ -3813,10 +3820,10 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="9" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B98" s="10" t="e">
-        <f aca="false">VLOOKUP(A98,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A98,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C98" s="9"/>
@@ -3846,10 +3853,10 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B99" s="10" t="e">
-        <f aca="false">VLOOKUP(A99,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A99,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C99" s="9"/>
@@ -3879,10 +3886,10 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B100" s="10" t="e">
-        <f aca="false">VLOOKUP(A100,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A100,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C100" s="9"/>
@@ -3912,10 +3919,10 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B101" s="10" t="e">
-        <f aca="false">VLOOKUP(A101,MAIN!A$1:D$1047791,4,0)</f>
+        <f aca="false">VLOOKUP(A101,MAIN!A$1:D$1047785,4,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C101" s="9"/>
@@ -3943,204 +3950,6 @@
       <c r="Y101" s="9"/>
       <c r="Z101" s="9"/>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B102" s="10" t="e">
-        <f aca="false">VLOOKUP(A102,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="9"/>
-      <c r="I102" s="9"/>
-      <c r="J102" s="9"/>
-      <c r="K102" s="9"/>
-      <c r="L102" s="9"/>
-      <c r="M102" s="9"/>
-      <c r="N102" s="9"/>
-      <c r="O102" s="9"/>
-      <c r="P102" s="9"/>
-      <c r="Q102" s="9"/>
-      <c r="R102" s="9"/>
-      <c r="S102" s="9"/>
-      <c r="T102" s="9"/>
-      <c r="U102" s="9"/>
-      <c r="V102" s="9"/>
-      <c r="W102" s="9"/>
-      <c r="X102" s="9"/>
-      <c r="Y102" s="9"/>
-      <c r="Z102" s="9"/>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B103" s="10" t="e">
-        <f aca="false">VLOOKUP(A103,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9"/>
-      <c r="F103" s="9"/>
-      <c r="G103" s="9"/>
-      <c r="H103" s="9"/>
-      <c r="I103" s="9"/>
-      <c r="J103" s="9"/>
-      <c r="K103" s="9"/>
-      <c r="L103" s="9"/>
-      <c r="M103" s="9"/>
-      <c r="N103" s="9"/>
-      <c r="O103" s="9"/>
-      <c r="P103" s="9"/>
-      <c r="Q103" s="9"/>
-      <c r="R103" s="9"/>
-      <c r="S103" s="9"/>
-      <c r="T103" s="9"/>
-      <c r="U103" s="9"/>
-      <c r="V103" s="9"/>
-      <c r="W103" s="9"/>
-      <c r="X103" s="9"/>
-      <c r="Y103" s="9"/>
-      <c r="Z103" s="9"/>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B104" s="10" t="e">
-        <f aca="false">VLOOKUP(A104,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="9"/>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-      <c r="M104" s="9"/>
-      <c r="N104" s="9"/>
-      <c r="O104" s="9"/>
-      <c r="P104" s="9"/>
-      <c r="Q104" s="9"/>
-      <c r="R104" s="9"/>
-      <c r="S104" s="9"/>
-      <c r="T104" s="9"/>
-      <c r="U104" s="9"/>
-      <c r="V104" s="9"/>
-      <c r="W104" s="9"/>
-      <c r="X104" s="9"/>
-      <c r="Y104" s="9"/>
-      <c r="Z104" s="9"/>
-    </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B105" s="10" t="e">
-        <f aca="false">VLOOKUP(A105,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C105" s="9"/>
-      <c r="D105" s="9"/>
-      <c r="E105" s="9"/>
-      <c r="F105" s="9"/>
-      <c r="G105" s="9"/>
-      <c r="H105" s="9"/>
-      <c r="I105" s="9"/>
-      <c r="J105" s="9"/>
-      <c r="K105" s="9"/>
-      <c r="L105" s="9"/>
-      <c r="M105" s="9"/>
-      <c r="N105" s="9"/>
-      <c r="O105" s="9"/>
-      <c r="P105" s="9"/>
-      <c r="Q105" s="9"/>
-      <c r="R105" s="9"/>
-      <c r="S105" s="9"/>
-      <c r="T105" s="9"/>
-      <c r="U105" s="9"/>
-      <c r="V105" s="9"/>
-      <c r="W105" s="9"/>
-      <c r="X105" s="9"/>
-      <c r="Y105" s="9"/>
-      <c r="Z105" s="9"/>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B106" s="10" t="e">
-        <f aca="false">VLOOKUP(A106,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C106" s="9"/>
-      <c r="D106" s="9"/>
-      <c r="E106" s="9"/>
-      <c r="F106" s="9"/>
-      <c r="G106" s="9"/>
-      <c r="H106" s="9"/>
-      <c r="I106" s="9"/>
-      <c r="J106" s="9"/>
-      <c r="K106" s="9"/>
-      <c r="L106" s="9"/>
-      <c r="M106" s="9"/>
-      <c r="N106" s="9"/>
-      <c r="O106" s="9"/>
-      <c r="P106" s="9"/>
-      <c r="Q106" s="9"/>
-      <c r="R106" s="9"/>
-      <c r="S106" s="9"/>
-      <c r="T106" s="9"/>
-      <c r="U106" s="9"/>
-      <c r="V106" s="9"/>
-      <c r="W106" s="9"/>
-      <c r="X106" s="9"/>
-      <c r="Y106" s="9"/>
-      <c r="Z106" s="9"/>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B107" s="10" t="e">
-        <f aca="false">VLOOKUP(A107,MAIN!A$1:D$1047791,4,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="9"/>
-      <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-      <c r="L107" s="9"/>
-      <c r="M107" s="9"/>
-      <c r="N107" s="9"/>
-      <c r="O107" s="9"/>
-      <c r="P107" s="9"/>
-      <c r="Q107" s="9"/>
-      <c r="R107" s="9"/>
-      <c r="S107" s="9"/>
-      <c r="T107" s="9"/>
-      <c r="U107" s="9"/>
-      <c r="V107" s="9"/>
-      <c r="W107" s="9"/>
-      <c r="X107" s="9"/>
-      <c r="Y107" s="9"/>
-      <c r="Z107" s="9"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>